<commit_message>
He renombrado ej8/index a indexPruebas porque estoy probando funciones
</commit_message>
<xml_diff>
--- a/Archivos/Funciones.xlsx
+++ b/Archivos/Funciones.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DES\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DC2A3D-F82D-4F89-A4F5-397C64D8B12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37F6666-0684-42A9-AFB8-7B6A0301E247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8315492C-99B7-4496-8BBA-6A10F97535C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8315492C-99B7-4496-8BBA-6A10F97535C8}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
     <sheet name="S" sheetId="3" r:id="rId2"/>
-    <sheet name="DATE" sheetId="5" r:id="rId3"/>
-    <sheet name="O" sheetId="4" r:id="rId4"/>
-    <sheet name="U" sheetId="2" r:id="rId5"/>
+    <sheet name="O" sheetId="4" r:id="rId3"/>
+    <sheet name="U" sheetId="2" r:id="rId4"/>
+    <sheet name="DATE" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>FUNCIONES</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>Para llamar a un elemento del array tendremos que poner el ($nombreArray)[$clave].</t>
+  </si>
+  <si>
+    <t>strtotime</t>
+  </si>
+  <si>
+    <t>Convierte una descripción de fecha/hora textual en Inglés a una fecha Unix</t>
+  </si>
+  <si>
+    <t>date([formato de la fecha], $timestamp (es un número entero, time())).                                                                      Por ejemplo                                                                          $fecha = "12/01/2003 17:52";                                                                     //utilizo strtotime para convertir la cadena a un entero que corresponde con la fecha/hora                            $fecha = strtotime(12/01/2003 17:52);                         echo $fecha (obtenemos =&gt; 1070297520);                        //Ahora ya hemos obtenido el timestamp (int) que necesitábamos para una fecha en concreto                                                               date("d/m/Y H:i:s", $fecha);</t>
+  </si>
+  <si>
+    <t>$fecha = strtotime(12/01/2003 17:52);                         echo $fecha (obtenemos =&gt; 1070297520);</t>
   </si>
 </sst>
 </file>
@@ -264,26 +276,26 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -306,16 +318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>55516</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>17416</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>768949</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>5035</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>730849</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>43135</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -338,7 +350,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10357756" y="167640"/>
+          <a:off x="11112136" y="38100"/>
           <a:ext cx="3090873" cy="3129235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -658,7 +670,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,27 +689,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -709,10 +709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22C9F0F-F9E4-4941-9DD8-DFF703F4E203}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,80 +752,34 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CCF04C-0835-4D58-92E3-D943C359D4B3}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="92.5546875" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="16"/>
-    </row>
-    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="16"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E203DD-BEC2-40CC-AD0D-ACC61D22C54F}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -876,12 +830,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81880F9F-E8BC-44FD-B21E-C015600B492D}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,4 +965,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CCF04C-0835-4D58-92E3-D943C359D4B3}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="92.5546875" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="159.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
"Añadida a array, la funcion array_intersect()"
</commit_message>
<xml_diff>
--- a/Archivos/Funciones.xlsx
+++ b/Archivos/Funciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DES\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D46ECEA-C32A-49B0-BA49-A4771157C93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BB6493-396C-4662-B79F-C37E7135BC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="11424" windowHeight="8964" activeTab="1" xr2:uid="{8315492C-99B7-4496-8BBA-6A10F97535C8}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="11424" windowHeight="8964" xr2:uid="{8315492C-99B7-4496-8BBA-6A10F97535C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="298">
   <si>
     <t>FUNCIONES</t>
   </si>
@@ -1955,6 +1955,30 @@
 echo strtr("hey, dije hola", $conv);
 ?&gt;
 hola, dije hey</t>
+  </si>
+  <si>
+    <t>array_intersect()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devuelve una matriz que contiene todos los valores array que están presentes en todos los 
+argumentos. Las claves se conservan. 
+El primer parámetro, es la matriz con los valores que queremos verificar.
+El segundo parámetro, son las matrices con las que vamos a comparar los valores anteriores.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;?php
+$array1 = array("a" =&gt; "green", "red", "blue");
+$array2 = array("b" =&gt; "green", "yellow", "red");
+$result = array_intersect($array1, $array2);
+print_r($result);
+?&gt;
+Formación
+(
+    [a] =&gt; verde
+    [0] =&gt; rojo
+)
+</t>
   </si>
 </sst>
 </file>
@@ -2217,6 +2241,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2226,12 +2262,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2239,12 +2269,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2619,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4C0BA5-67CA-4BF0-AF87-5886AC2AB380}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3037,7 +3061,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="360" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>125</v>
       </c>
@@ -3084,20 +3108,20 @@
       <c r="C42" s="22"/>
     </row>
     <row r="43" spans="1:4" ht="259.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="28" t="s">
         <v>134</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="30" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="303" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="27"/>
-      <c r="C44" s="32"/>
+      <c r="C44" s="31"/>
     </row>
     <row r="45" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
@@ -3176,10 +3200,16 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="8"/>
+    <row r="52" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
@@ -3223,7 +3253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15781DA7-1F29-4D25-BD3A-E2070CCC16C8}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -3766,47 +3796,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="159.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="32"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" s="11"/>
@@ -3841,10 +3871,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3872,20 +3902,20 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="32"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3913,10 +3943,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3964,10 +3994,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>